<commit_message>
Changed database filtering logic to include all plants
</commit_message>
<xml_diff>
--- a/LCOH modelling/data/facility_temps.xlsx
+++ b/LCOH modelling/data/facility_temps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antoine\Desktop\LCOH modelling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antoine\Desktop\LCOH modelling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C8DDD4-CE26-4839-B424-94AB00645B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6950B24-EC85-4B2C-808D-B20ADF2990E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="444" yWindow="1140" windowWidth="21600" windowHeight="11100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAICS" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,10 @@
     <t>temperature</t>
   </si>
   <si>
-    <t>facility_id</t>
+    <t>primary_naics</t>
   </si>
   <si>
-    <t>primary_naics</t>
+    <t>facility_id</t>
   </si>
 </sst>
 </file>
@@ -362,7 +362,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -401,7 +401,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>

</xml_diff>